<commit_message>
removed student update only with 5 hours
</commit_message>
<xml_diff>
--- a/utils/uploads/attendanceSheet (1).xlsx
+++ b/utils/uploads/attendanceSheet (1).xlsx
@@ -19,9 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>AC PRIMARY SCHOOL II, BAGIDO</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="99">
+  <si>
+    <t>LOCAL GOVERNMENT EDUCATION AUTHORITY CATHOLIC PRIMARY SCHOOL, KARAWORO</t>
   </si>
   <si>
     <t>S/N</t>
@@ -45,19 +45,277 @@
     <t>AttendanceScore</t>
   </si>
   <si>
-    <t>jDEsUuUeV</t>
-  </si>
-  <si>
-    <t>Joseph</t>
-  </si>
-  <si>
-    <t>Famous</t>
-  </si>
-  <si>
-    <t>Emeka</t>
+    <t>vywKGWhK9</t>
+  </si>
+  <si>
+    <t>Onwubalili</t>
+  </si>
+  <si>
+    <t>Nzube</t>
+  </si>
+  <si>
+    <t>Phili</t>
+  </si>
+  <si>
+    <t>SSS 1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>vywKGWhA1</t>
+  </si>
+  <si>
+    <t>r1a9QyZpX</t>
+  </si>
+  <si>
+    <t>s3aZy6QdX</t>
+  </si>
+  <si>
+    <t>P9uD8V3kJ</t>
+  </si>
+  <si>
+    <t>D8rM5S1xK</t>
+  </si>
+  <si>
+    <t>M1dF9B2kL</t>
+  </si>
+  <si>
+    <t>Q8nH2Y4zP</t>
+  </si>
+  <si>
+    <t>Adediran</t>
+  </si>
+  <si>
+    <t>Oluwaseun</t>
+  </si>
+  <si>
+    <t>Adebayo</t>
   </si>
   <si>
     <t>JSS 3</t>
+  </si>
+  <si>
+    <t>T9lF3S2qV</t>
+  </si>
+  <si>
+    <t>Okafor</t>
+  </si>
+  <si>
+    <t>Chinonso</t>
+  </si>
+  <si>
+    <t>Ngozi</t>
+  </si>
+  <si>
+    <t>Z8oK5C7nW</t>
+  </si>
+  <si>
+    <t>Ibrahim</t>
+  </si>
+  <si>
+    <t>Olamide</t>
+  </si>
+  <si>
+    <t>Tariq</t>
+  </si>
+  <si>
+    <t>Primary 6</t>
+  </si>
+  <si>
+    <t>U1gL7J6bZ</t>
+  </si>
+  <si>
+    <t>Bello</t>
+  </si>
+  <si>
+    <t>Zainab</t>
+  </si>
+  <si>
+    <t>Fatimah</t>
+  </si>
+  <si>
+    <t>JSS 1</t>
+  </si>
+  <si>
+    <t>P7bI9F2mQ</t>
+  </si>
+  <si>
+    <t>Adeyemo</t>
+  </si>
+  <si>
+    <t>Bolanle</t>
+  </si>
+  <si>
+    <t>Jibola</t>
+  </si>
+  <si>
+    <t>F8gJ3N5aX</t>
+  </si>
+  <si>
+    <t>Akinpelu</t>
+  </si>
+  <si>
+    <t>Temidayo</t>
+  </si>
+  <si>
+    <t>B4jD1L0rV</t>
+  </si>
+  <si>
+    <t>Sule</t>
+  </si>
+  <si>
+    <t>Abdulrahman</t>
+  </si>
+  <si>
+    <t>Micheal</t>
+  </si>
+  <si>
+    <t>A2lF9Q6rX</t>
+  </si>
+  <si>
+    <t>Olumide</t>
+  </si>
+  <si>
+    <t>Temiloluwa</t>
+  </si>
+  <si>
+    <t>G7hK8R4iP</t>
+  </si>
+  <si>
+    <t>Bamidele</t>
+  </si>
+  <si>
+    <t>Adedayo</t>
+  </si>
+  <si>
+    <t>Ruth</t>
+  </si>
+  <si>
+    <t>L9kW5O8nD</t>
+  </si>
+  <si>
+    <t>Akintoye</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>B2mW4C5kT</t>
+  </si>
+  <si>
+    <t>Emmanuel</t>
+  </si>
+  <si>
+    <t>T2yD4R8nF</t>
+  </si>
+  <si>
+    <t>Adeleke</t>
+  </si>
+  <si>
+    <t>Adewale</t>
+  </si>
+  <si>
+    <t>Taiwo</t>
+  </si>
+  <si>
+    <t>N2kL5R7hP</t>
+  </si>
+  <si>
+    <t>Sulaimon</t>
+  </si>
+  <si>
+    <t>Muhammad</t>
+  </si>
+  <si>
+    <t>O2gP9Y3rJ</t>
+  </si>
+  <si>
+    <t>Durojaiye</t>
+  </si>
+  <si>
+    <t>Babatunde</t>
+  </si>
+  <si>
+    <t>B4pT2Q8hM</t>
+  </si>
+  <si>
+    <t>Amina</t>
+  </si>
+  <si>
+    <t>S5iU3B2mL</t>
+  </si>
+  <si>
+    <t>Seyi</t>
+  </si>
+  <si>
+    <t>Tobiloba</t>
+  </si>
+  <si>
+    <t>W3oP6J2kD</t>
+  </si>
+  <si>
+    <t>Olawale</t>
+  </si>
+  <si>
+    <t>Ademola</t>
+  </si>
+  <si>
+    <t>Z7kL1T9hN</t>
+  </si>
+  <si>
+    <t>Nwankwo</t>
+  </si>
+  <si>
+    <t>Chijioke</t>
+  </si>
+  <si>
+    <t>Q1pD9R6wZ</t>
+  </si>
+  <si>
+    <t>Adeola</t>
+  </si>
+  <si>
+    <t>Oluwatobiloba</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>G3fA7E2vK</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Oluwadamilola</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>H9fE2S5rJ</t>
+  </si>
+  <si>
+    <t>Salami</t>
+  </si>
+  <si>
+    <t>Y9kFAAEZo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philip </t>
+  </si>
+  <si>
+    <t>8FDV9ZQCU</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
 </sst>
 </file>
@@ -435,15 +693,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="15.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +715,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -474,7 +738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -494,7 +758,674 @@
         <v>12</v>
       </c>
       <c r="G4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>98</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -503,7 +1434,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G3 A4:F4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G3 A5:F33 A4:F4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>